<commit_message>
Updated documentation, input files and input reader
Signed-off-by: Aytug Yavuzer <aytug.yavuzer@rwth-aachen.de>
</commit_message>
<xml_diff>
--- a/src/tutorials/scenario_generation/input_generator_conditional_pdfs.xlsx
+++ b/src/tutorials/scenario_generation/input_generator_conditional_pdfs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aytugy\Desktop\workspace\datafev\src\tutorials\scenario_generation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E33248B-9A5B-4229-8623-B9F7D71C8486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A603CF5C-55DA-4581-9799-95FE53AB6EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{6D84608D-2842-4D80-A276-F6871E651D14}"/>
+    <workbookView minimized="1" xWindow="2445" yWindow="1830" windowWidth="21600" windowHeight="11295" activeTab="4" xr2:uid="{6D84608D-2842-4D80-A276-F6871E651D14}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeID" sheetId="1" r:id="rId1"/>
@@ -54,27 +54,12 @@
     <t>SoCID</t>
   </si>
   <si>
-    <t>SoCLowerBound</t>
-  </si>
-  <si>
-    <t>SoCUpperBound</t>
-  </si>
-  <si>
     <t>Probability</t>
   </si>
   <si>
     <t>Model</t>
   </si>
   <si>
-    <t>BatteryCapacity</t>
-  </si>
-  <si>
-    <t>MaxChargingPower</t>
-  </si>
-  <si>
-    <t>MaxFastChargingPower</t>
-  </si>
-  <si>
     <t>honda e</t>
   </si>
   <si>
@@ -133,6 +118,21 @@
   </si>
   <si>
     <t>audi e-tron gt rs</t>
+  </si>
+  <si>
+    <t>SoCLowerBound(%)</t>
+  </si>
+  <si>
+    <t>SoCUpperBound(%)</t>
+  </si>
+  <si>
+    <t>BatteryCapacity(kWh)</t>
+  </si>
+  <si>
+    <t>MaxChargingPower(kW)</t>
+  </si>
+  <si>
+    <t>MaxFastChargingPower(kW)</t>
   </si>
 </sst>
 </file>
@@ -770,7 +770,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,10 +783,10 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -842,7 +842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34DF8125-BA3D-476F-862D-6A92E0D3D976}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -942,39 +942,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B16D92-4B1C-4569-86C9-CA691277B308}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>28.5</v>
@@ -991,7 +991,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>75</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>57.5</v>
@@ -1025,7 +1025,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>75</v>
@@ -1042,7 +1042,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>80.7</v>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>107.8</v>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>74</v>
@@ -1093,7 +1093,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>60</v>
@@ -1110,7 +1110,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>87</v>
@@ -1127,7 +1127,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>64.8</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>77</v>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>90.6</v>
@@ -1178,7 +1178,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>105.2</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>64</v>
@@ -1212,7 +1212,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>71</v>
@@ -1229,7 +1229,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>74</v>
@@ -1246,7 +1246,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B18">
         <v>95</v>
@@ -1263,7 +1263,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>107.8</v>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B20">
         <v>80.7</v>
@@ -1297,7 +1297,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B21">
         <v>85</v>

</xml_diff>